<commit_message>
Entrega do projeto para coleção de Inverno
</commit_message>
<xml_diff>
--- a/categorias.xlsx
+++ b/categorias.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.cristiano\Documents\GitHub\Upload-catalogo-de-produtos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBACFEB1-9A06-4F3C-BD49-B91B01FB5297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF16D1AE-CCD7-42A6-A192-F6732DEF88D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C9FFF442-299F-4692-8143-443A0FDD541E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>CALÇADO</t>
   </si>
@@ -79,6 +79,27 @@
   </si>
   <si>
     <t>CATEGORIA</t>
+  </si>
+  <si>
+    <t>JERSEY</t>
+  </si>
+  <si>
+    <t>CAMISA</t>
+  </si>
+  <si>
+    <t>REGATA</t>
+  </si>
+  <si>
+    <t>SAIA</t>
+  </si>
+  <si>
+    <t>VESTIDO</t>
+  </si>
+  <si>
+    <t>CUECA</t>
+  </si>
+  <si>
+    <t>TOP</t>
   </si>
 </sst>
 </file>
@@ -116,7 +137,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,143 +452,143 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B2ECCAE-C01F-40AE-AB78-0E5059AEC585}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>17</v>
       </c>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>19</v>
       </c>
     </row>
@@ -575,8 +596,64 @@
       <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>